<commit_message>
Add power consumption via UPS Hat on Zero W
</commit_message>
<xml_diff>
--- a/doc/power_consumption.xlsx
+++ b/doc/power_consumption.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">Power Consumption</t>
   </si>
   <si>
-    <t xml:space="preserve">mA @ 5V</t>
+    <t xml:space="preserve">mA</t>
   </si>
   <si>
     <t xml:space="preserve">Wh</t>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Playing</t>
   </si>
   <si>
+    <t xml:space="preserve">@V</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPi 4B with built-in audio out</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">RPi Zero W with HifiBerry DAC Zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPi Zero W, HifiBerry DAC Zero, UPS Hat</t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +218,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,14 +254,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,7 +270,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,573 +457,635 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="18.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.26"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="G4" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="8" t="n">
+      <c r="H4" s="9" t="n">
         <v>1000</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="I4" s="9" t="n">
         <v>3000</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="J4" s="9" t="n">
         <v>6600</v>
       </c>
-      <c r="J4" s="10" t="n">
+      <c r="K4" s="11" t="n">
         <v>10000</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B5" s="12" t="n">
         <v>470</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>480</v>
       </c>
-      <c r="D5" s="12" t="n">
-        <f aca="false">B5/1000*5</f>
+      <c r="D5" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="14" t="n">
+        <f aca="false">B5/1000*$D5</f>
         <v>2.35</v>
       </c>
-      <c r="E5" s="13" t="n">
-        <f aca="false">C5/1000*5</f>
+      <c r="F5" s="14" t="n">
+        <f aca="false">C5/1000*$D5</f>
         <v>2.4</v>
       </c>
-      <c r="F5" s="14" t="n">
-        <f aca="false">E5*(1+F$4/100)</f>
+      <c r="G5" s="15" t="n">
+        <f aca="false">F5*(1+G$4/100)</f>
         <v>2.64</v>
       </c>
-      <c r="G5" s="13" t="n">
-        <f aca="false">((G$4/1000*3.7)/$F5)</f>
+      <c r="H5" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G5)</f>
         <v>1.40151515151515</v>
       </c>
-      <c r="H5" s="13" t="n">
-        <f aca="false">((H$4/1000*3.7)/$F5)</f>
+      <c r="I5" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G5)</f>
         <v>4.20454545454546</v>
       </c>
-      <c r="I5" s="13" t="n">
-        <f aca="false">((I$4/1000*3.7)/$F5)</f>
+      <c r="J5" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G5)</f>
         <v>9.25</v>
       </c>
-      <c r="J5" s="15" t="n">
-        <f aca="false">((J$4/1000*3.7)/$F5)</f>
+      <c r="K5" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G5)</f>
         <v>14.0151515151515</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B6" s="12" t="n">
         <v>940</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="D6" s="12" t="n">
-        <f aca="false">B6/1000*5</f>
+      <c r="D6" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <f aca="false">B6/1000*$D6</f>
         <v>4.7</v>
       </c>
-      <c r="E6" s="13" t="n">
-        <f aca="false">C6/1000*5</f>
+      <c r="F6" s="14" t="n">
+        <f aca="false">C6/1000*$D6</f>
         <v>5</v>
       </c>
-      <c r="F6" s="14" t="n">
-        <f aca="false">E6*(1+F$4/100)</f>
+      <c r="G6" s="15" t="n">
+        <f aca="false">F6*(1+G$4/100)</f>
         <v>5.5</v>
       </c>
-      <c r="G6" s="13" t="n">
-        <f aca="false">((G$4/1000*3.7)/$F6)</f>
+      <c r="H6" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G6)</f>
         <v>0.672727272727273</v>
       </c>
-      <c r="H6" s="13" t="n">
-        <f aca="false">((H$4/1000*3.7)/$F6)</f>
+      <c r="I6" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G6)</f>
         <v>2.01818181818182</v>
       </c>
-      <c r="I6" s="13" t="n">
-        <f aca="false">((I$4/1000*3.7)/$F6)</f>
+      <c r="J6" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G6)</f>
         <v>4.44</v>
       </c>
-      <c r="J6" s="15" t="n">
-        <f aca="false">((J$4/1000*3.7)/$F6)</f>
+      <c r="K6" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G6)</f>
         <v>6.72727272727273</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B7" s="12" t="n">
         <v>100</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="D7" s="12" t="n">
-        <f aca="false">B7/1000*5</f>
+      <c r="D7" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <f aca="false">B7/1000*$D7</f>
         <v>0.5</v>
       </c>
-      <c r="E7" s="13" t="n">
-        <f aca="false">C7/1000*5</f>
+      <c r="F7" s="14" t="n">
+        <f aca="false">C7/1000*$D7</f>
         <v>0.55</v>
       </c>
-      <c r="F7" s="14" t="n">
-        <f aca="false">E7*(1+F$4/100)</f>
+      <c r="G7" s="15" t="n">
+        <f aca="false">F7*(1+G$4/100)</f>
         <v>0.605</v>
       </c>
-      <c r="G7" s="13" t="n">
-        <f aca="false">((G$4/1000*3.7)/$F7)</f>
+      <c r="H7" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G7)</f>
         <v>6.11570247933884</v>
       </c>
-      <c r="H7" s="13" t="n">
-        <f aca="false">((H$4/1000*3.7)/$F7)</f>
+      <c r="I7" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G7)</f>
         <v>18.3471074380165</v>
       </c>
-      <c r="I7" s="13" t="n">
-        <f aca="false">((I$4/1000*3.7)/$F7)</f>
+      <c r="J7" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G7)</f>
         <v>40.3636363636364</v>
       </c>
-      <c r="J7" s="15" t="n">
-        <f aca="false">((J$4/1000*3.7)/$F7)</f>
+      <c r="K7" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G7)</f>
         <v>61.1570247933884</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" s="12" t="n">
         <v>110</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="D8" s="12" t="n">
-        <f aca="false">B8/1000*5</f>
+      <c r="D8" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <f aca="false">B8/1000*$D8</f>
         <v>0.55</v>
       </c>
-      <c r="E8" s="13" t="n">
-        <f aca="false">C8/1000*5</f>
+      <c r="F8" s="14" t="n">
+        <f aca="false">C8/1000*$D8</f>
         <v>0.7</v>
       </c>
-      <c r="F8" s="14" t="n">
-        <f aca="false">E8*(1+F$4/100)</f>
+      <c r="G8" s="15" t="n">
+        <f aca="false">F8*(1+G$4/100)</f>
         <v>0.77</v>
       </c>
-      <c r="G8" s="13" t="n">
-        <f aca="false">((G$4/1000*3.7)/$F8)</f>
+      <c r="H8" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G8)</f>
         <v>4.8051948051948</v>
       </c>
-      <c r="H8" s="13" t="n">
-        <f aca="false">((H$4/1000*3.7)/$F8)</f>
+      <c r="I8" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G8)</f>
         <v>14.4155844155844</v>
       </c>
-      <c r="I8" s="13" t="n">
-        <f aca="false">((I$4/1000*3.7)/$F8)</f>
+      <c r="J8" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G8)</f>
         <v>31.7142857142857</v>
       </c>
-      <c r="J8" s="15" t="n">
-        <f aca="false">((J$4/1000*3.7)/$F8)</f>
+      <c r="K8" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G8)</f>
         <v>48.051948051948</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="16"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="15"/>
-    </row>
-    <row r="10" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="16"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="13"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="12" t="n">
+        <v>160</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D9" s="17" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <f aca="false">B9/1000*$D9</f>
+        <v>0.592</v>
+      </c>
+      <c r="F9" s="14" t="n">
+        <f aca="false">C9/1000*$D9</f>
+        <v>0.74</v>
+      </c>
+      <c r="G9" s="15" t="n">
+        <f aca="false">F9*(1+G$4/100)</f>
+        <v>0.814</v>
+      </c>
+      <c r="H9" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G9)</f>
+        <v>4.54545454545455</v>
+      </c>
+      <c r="I9" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G9)</f>
+        <v>13.6363636363636</v>
+      </c>
+      <c r="J9" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G9)</f>
+        <v>30</v>
+      </c>
+      <c r="K9" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G9)</f>
+        <v>45.4545454545454</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="12"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="15"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="16"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="12"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="15"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="16"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="12"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="15"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="15"/>
-    </row>
-    <row r="13" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="16"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="12"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="15"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="16"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="12"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="16"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="12"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="16"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="12"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="16"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="12"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="15"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="16"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="12"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="16"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="12"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="16"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="12"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="15"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="16"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="12"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="15"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="12"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="15"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
-    </row>
-    <row r="24" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
-    </row>
-    <row r="25" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
-    </row>
-    <row r="26" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
-    </row>
-    <row r="27" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="13"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
-    </row>
-    <row r="28" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="13"/>
+      <c r="K27" s="13"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
-    </row>
-    <row r="29" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="13"/>
+      <c r="K28" s="13"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
-    </row>
-    <row r="30" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="13"/>
+      <c r="K29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
-    </row>
-    <row r="31" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="13"/>
+      <c r="K30" s="13"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
-    </row>
-    <row r="32" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="13"/>
+      <c r="K31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
-    </row>
-    <row r="33" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="13"/>
+      <c r="K32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
-    </row>
-    <row r="34" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="13"/>
+      <c r="K33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="13"/>
+      <c r="K34" s="13"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
-    </row>
-    <row r="36" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="13"/>
+      <c r="K35" s="13"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
-    </row>
-    <row r="37" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="13"/>
+      <c r="K36" s="13"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
-    </row>
-    <row r="38" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="13"/>
+      <c r="K37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
-    </row>
-    <row r="39" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="13"/>
+      <c r="K38" s="13"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
-    </row>
-    <row r="40" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="13"/>
+      <c r="K39" s="13"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
-    </row>
-    <row r="41" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="13"/>
+      <c r="K40" s="13"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
-    </row>
-    <row r="42" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="13"/>
+      <c r="K41" s="13"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="13"/>
+      <c r="K42" s="13"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
-    </row>
-    <row r="44" customFormat="false" ht="18.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="13"/>
+      <c r="K43" s="13"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="H3:K3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add power consumption with MiniAMP board and speakers
</commit_message>
<xml_diff>
--- a/doc/power_consumption.xlsx
+++ b/doc/power_consumption.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Power Consumption</t>
   </si>
@@ -62,6 +62,21 @@
   </si>
   <si>
     <t xml:space="preserve">RPi Zero W, HifiBerry DAC Zero, UPS Hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPi Zero W, MiniAMP, UPS Hat – No Speaker, 100% Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPi Zero W, MiniAMP, UPS Hat – 1 Speaker, 50% Volume, Over the Rainbow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPi Zero W, MiniAMP, UPS Hat – 1 Speaker, 50% Volume, 120Hz Sine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPi Zero W, MiniAMP, UPS Hat – 2 Speakers, 100% Volume, O. t. Rainbow, AVG!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPi Zero W, MiniAMP, UPS Hat – 2 Speakers, 100% Volume, 120Hz Sine</t>
   </si>
 </sst>
 </file>
@@ -201,7 +216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -267,10 +282,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,14 +471,13 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="70.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.26"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,10 +715,10 @@
       <c r="B9" s="12" t="n">
         <v>160</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="D9" s="17" t="n">
+      <c r="D9" s="13" t="n">
         <v>3.7</v>
       </c>
       <c r="E9" s="14" t="n">
@@ -741,63 +751,218 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="12" t="n">
+        <v>180</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E10" s="14" t="n">
+        <f aca="false">B10/1000*$D10</f>
+        <v>0.666</v>
+      </c>
+      <c r="F10" s="14" t="n">
+        <f aca="false">C10/1000*$D10</f>
+        <v>0.888</v>
+      </c>
+      <c r="G10" s="15" t="n">
+        <f aca="false">F10*(1+G$4/100)</f>
+        <v>0.9768</v>
+      </c>
+      <c r="H10" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G10)</f>
+        <v>3.78787878787879</v>
+      </c>
+      <c r="I10" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G10)</f>
+        <v>11.3636363636364</v>
+      </c>
+      <c r="J10" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G10)</f>
+        <v>25</v>
+      </c>
+      <c r="K10" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G10)</f>
+        <v>37.8787878787879</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="16"/>
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="12" t="n">
+        <v>180</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="D11" s="13" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E11" s="14" t="n">
+        <f aca="false">B11/1000*$D11</f>
+        <v>0.666</v>
+      </c>
+      <c r="F11" s="14" t="n">
+        <f aca="false">C11/1000*$D11</f>
+        <v>0.925</v>
+      </c>
+      <c r="G11" s="15" t="n">
+        <f aca="false">F11*(1+G$4/100)</f>
+        <v>1.0175</v>
+      </c>
+      <c r="H11" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G11)</f>
+        <v>3.63636363636364</v>
+      </c>
+      <c r="I11" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G11)</f>
+        <v>10.9090909090909</v>
+      </c>
+      <c r="J11" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G11)</f>
+        <v>24</v>
+      </c>
+      <c r="K11" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G11)</f>
+        <v>36.3636363636364</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="16"/>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="12" t="n">
+        <v>180</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>450</v>
+      </c>
+      <c r="D12" s="13" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E12" s="14" t="n">
+        <f aca="false">B12/1000*$D12</f>
+        <v>0.666</v>
+      </c>
+      <c r="F12" s="14" t="n">
+        <f aca="false">C12/1000*$D12</f>
+        <v>1.665</v>
+      </c>
+      <c r="G12" s="15" t="n">
+        <f aca="false">F12*(1+G$4/100)</f>
+        <v>1.8315</v>
+      </c>
+      <c r="H12" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G12)</f>
+        <v>2.02020202020202</v>
+      </c>
+      <c r="I12" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G12)</f>
+        <v>6.06060606060606</v>
+      </c>
+      <c r="J12" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G12)</f>
+        <v>13.3333333333333</v>
+      </c>
+      <c r="K12" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G12)</f>
+        <v>20.2020202020202</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="16"/>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="12" t="n">
+        <v>180</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <f aca="false">B13/1000*$D13</f>
+        <v>0.666</v>
+      </c>
+      <c r="F13" s="14" t="n">
+        <f aca="false">C13/1000*$D13</f>
+        <v>2.59</v>
+      </c>
+      <c r="G13" s="15" t="n">
+        <f aca="false">F13*(1+G$4/100)</f>
+        <v>2.849</v>
+      </c>
+      <c r="H13" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G13)</f>
+        <v>1.2987012987013</v>
+      </c>
+      <c r="I13" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G13)</f>
+        <v>3.8961038961039</v>
+      </c>
+      <c r="J13" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G13)</f>
+        <v>8.57142857142857</v>
+      </c>
+      <c r="K13" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G13)</f>
+        <v>12.987012987013</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="16"/>
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="12" t="n">
+        <v>180</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1260</v>
+      </c>
+      <c r="D14" s="13" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="E14" s="14" t="n">
+        <f aca="false">B14/1000*$D14</f>
+        <v>0.666</v>
+      </c>
+      <c r="F14" s="14" t="n">
+        <f aca="false">C14/1000*$D14</f>
+        <v>4.662</v>
+      </c>
+      <c r="G14" s="15" t="n">
+        <f aca="false">F14*(1+G$4/100)</f>
+        <v>5.1282</v>
+      </c>
+      <c r="H14" s="13" t="n">
+        <f aca="false">((H$4/1000*3.7)/$G14)</f>
+        <v>0.721500721500721</v>
+      </c>
+      <c r="I14" s="13" t="n">
+        <f aca="false">((I$4/1000*3.7)/$G14)</f>
+        <v>2.16450216450216</v>
+      </c>
+      <c r="J14" s="13" t="n">
+        <f aca="false">((J$4/1000*3.7)/$G14)</f>
+        <v>4.76190476190476</v>
+      </c>
+      <c r="K14" s="16" t="n">
+        <f aca="false">((K$4/1000*3.7)/$G14)</f>
+        <v>7.21500721500722</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="12"/>
-      <c r="D15" s="17"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
@@ -808,7 +973,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="12"/>
-      <c r="D16" s="17"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
@@ -819,7 +984,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="12"/>
-      <c r="D17" s="17"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="14"/>
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
@@ -830,7 +995,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="12"/>
-      <c r="D18" s="17"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="14"/>
       <c r="F18" s="13"/>
       <c r="G18" s="15"/>
@@ -841,7 +1006,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="12"/>
-      <c r="D19" s="17"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="14"/>
       <c r="F19" s="13"/>
       <c r="G19" s="15"/>
@@ -852,7 +1017,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="12"/>
-      <c r="D20" s="17"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="14"/>
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
@@ -863,7 +1028,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="12"/>
-      <c r="D21" s="17"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="14"/>
       <c r="F21" s="13"/>
       <c r="G21" s="15"/>
@@ -874,7 +1039,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="12"/>
-      <c r="D22" s="17"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="14"/>
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>

</xml_diff>